<commit_message>
Implemented teachers and their subjects
</commit_message>
<xml_diff>
--- a/sheet_engine/static/template_sheets/teacher_subjects.xlsx
+++ b/sheet_engine/static/template_sheets/teacher_subjects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeLab\Projects\curie\sheet_engine\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeLab\Projects\curie\sheet_engine\static\template_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57A9F98-F2F3-4316-BB29-59498C3D5BCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAB5892-5E56-45FC-AF14-85FE4B9912A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1650" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="teacher_subjects" sheetId="1" r:id="rId1"/>
@@ -99,13 +99,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,140 +512,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -657,14 +657,14 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
@@ -676,27 +676,27 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>5</v>

</xml_diff>